<commit_message>
release pilgrimage and trust
</commit_message>
<xml_diff>
--- a/trust/StructureDefinition-COSEHeader.xlsx
+++ b/trust/StructureDefinition-COSEHeader.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.2</t>
+    <t>1.1.3</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-12T08:01:09+00:00</t>
+    <t>2024-04-25T23:34:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>